<commit_message>
added Active Cases graph
</commit_message>
<xml_diff>
--- a/testing/covid-testing-latest-data-source-details.xlsx
+++ b/testing/covid-testing-latest-data-source-details.xlsx
@@ -77,7 +77,7 @@
     <t xml:space="preserve">Argentina - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/30-04-20_reporte_matutino_covid_19.pdf</t>
+    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/09-05-20_reporte-matutino-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Argentina</t>
@@ -98,7 +98,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/05/coronavirus-covid-19-at-a-glance-6-may-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/05/coronavirus-covid-19-at-a-glance-9-may-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -118,7 +118,7 @@
     <t xml:space="preserve">Austria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506175135/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510104642/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
   </si>
   <si>
     <t xml:space="preserve">Austrian Ministry for Health</t>
@@ -145,7 +145,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506175139/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200509192849/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -193,7 +193,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-na-4-maya-vyzdoroveli-i-vypisany-3259-patsientov/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-na-8-maya-vyzdoroveli-i-vypisany-5-tys-484-patsienta/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -247,7 +247,7 @@
   </si>
   <si>
     <t xml:space="preserve">Official testing data from the Bolivian Ministry of Health is reported in [this dashboard](https://www.boliviasegura.gob.bo/datos-oficiales), which provides a breakdown of the cumulative number of confirmed, suspected, and discarded cases to date along with the number of deaths and recoveries. We assume that the number of discarded cases ("casos descartados") refers to the number of cases with negative test results. Under this assumption, we measure the total number of cases tested to date as the sum of the number of confirmed and discarded cases.
-Unfortunately, the official dashboard does not provide a time series of the number of cases tested each day since testing began. Instead, the dashboard only displays a daily snapshot of the total cases tested to date. Since we did not begin monitoring this dashboard until April 15th 2020, we construct a time series dating back to March 21st 2020 using data provided in [this unofficial Github repository](https://github.com/mauforonda/covid19-bolivia), which we have cross-referenced against data in the official dashboard for a sample of dates.</t>
+Unfortunately, the official dashboard does not provide a time series of the number of cases tested each day since testing began. Instead, the dashboard only displays a daily snapshot of the total cases tested to date. Since we did not begin monitoring this dashboard until April 15th 2020, we construct a time series dating back to March 21st 2020 using data provided in [this unofficial GitHub repository](https://github.com/mauforonda/covid19-bolivia), which we have cross-referenced against data in the official dashboard for a sample of dates.</t>
   </si>
   <si>
     <t xml:space="preserve">BRA</t>
@@ -277,7 +277,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506175144/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510104647/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -300,7 +300,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506175147/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510104649/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -336,13 +336,13 @@
     <t xml:space="preserve">https://www.gob.cl/coronavirus/cifrasoficiales/#reportes</t>
   </si>
   <si>
-    <t xml:space="preserve">The Government of Chile release daily reports that include cumulative and daily totals for the number of PCR tests performed across private and public medical establishments. This data is collected by volunteers and [published on Github](https://github.com/jorgeperezrojas/covid19-data). We take our figures from this GitHub, which we regularly audit for accuracy.</t>
+    <t xml:space="preserve">The Government of Chile release daily reports that include cumulative and daily totals for the number of PCR tests performed across private and public medical establishments. This data is collected by volunteers and [published on GitHub](https://github.com/jorgeperezrojas/covid19-data). We take our figures from this GitHub, which we regularly audit for accuracy.</t>
   </si>
   <si>
     <t xml:space="preserve">COL</t>
   </si>
   <si>
-    <t xml:space="preserve">Colombia - samples processed</t>
+    <t xml:space="preserve">Colombia - samples tested</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.ins.gov.co/Noticias/Paginas/Coronavirus.aspx#muestras</t>
@@ -388,7 +388,7 @@
     <t xml:space="preserve">Croatia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506175452/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200509164031/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Croatia</t>
@@ -445,10 +445,10 @@
     <t xml:space="preserve">DNK</t>
   </si>
   <si>
-    <t xml:space="preserve">Denmark - People tested</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://files.ssi.dk/COVID19-overvaagningsrapport-06052020-pp5f</t>
+    <t xml:space="preserve">Denmark - people tested</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://files.ssi.dk/COVID19-overvaagningsrapport-09052020-hu51</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -475,7 +475,7 @@
     <t xml:space="preserve">Ecuador - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/05/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-04052020-08h00.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/05/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-08052020-08h0.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -504,7 +504,7 @@
     <t xml:space="preserve">Government of El Salvador</t>
   </si>
   <si>
-    <t xml:space="preserve">updated at 12:10am local time on 2020-05-06.</t>
+    <t xml:space="preserve">updated at 12:50pm local time on 2020-05-09.</t>
   </si>
   <si>
     <t xml:space="preserve">The government of El Salvador publishes an online dashboard with figures and graphs about the epidemic, including the number of tests performed ("pruebas COVID19 realizadas hasta hoy"). No information is given on the geographical scope and number of labs included.</t>
@@ -541,7 +541,7 @@
     <t xml:space="preserve">Ethiopia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_May-6_-ENG-V4-1.pdf</t>
+    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_May-8_-ENG-V5.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ethiopian Public Health Institute</t>
@@ -585,7 +585,7 @@
     <t xml:space="preserve">France - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.santepubliquefrance.fr/content/download/249184/2589560</t>
+    <t xml:space="preserve">https://www.santepubliquefrance.fr/content/download/250807/2596023</t>
   </si>
   <si>
     <t xml:space="preserve">Agence nationale de santé publique</t>
@@ -669,7 +669,7 @@
     <t xml:space="preserve">Greece - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200506/</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200509/</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -739,7 +739,7 @@
     <t xml:space="preserve">ISL</t>
   </si>
   <si>
-    <t xml:space="preserve">Iceland - samples</t>
+    <t xml:space="preserve">Iceland - samples tested</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.covid.is/tolulegar-upplysingar</t>
@@ -771,7 +771,7 @@
   </si>
   <si>
     <t xml:space="preserve">The ICMR reports separate figures for both “samples tested” and “people tested” at press conferences and in press releases (shown separately in the charts above). No other details are provided.
-The press releases from ICMR do not always stay online for very long. The reason for this is unknown, but the releases are being backed up at this [Github repository](https://github.com/datameet/covid19).
+The press releases from ICMR do not always stay online for very long. The reason for this is unknown, but the releases are being backed up at this [GitHub repository](https://github.com/datameet/covid19).
 On some occasions there appear to have been more than one update released per day. Where we are aware of multiple observations for the day, we show the number for the earlier release.</t>
   </si>
   <si>
@@ -804,7 +804,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200506141329/http://irangov.ir/detail/338787</t>
+    <t xml:space="preserve">http://web.archive.org/web/20200509000642/http://irangov.ir/detail/338857</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -856,7 +856,7 @@
     <t xml:space="preserve">https://t.me/s/MOHreport</t>
   </si>
   <si>
-    <t xml:space="preserve">The Israel Ministry of Health publishes COVID-19 updates on its official channel on Telegram. This data is published in a format that is extremely challenging to collect. We rely on the data as collected and made available [on Github](https://github.com/idandrd/israel-covid19-data/blob/master/Corona-Tests.csv).
+    <t xml:space="preserve">The Israel Ministry of Health publishes COVID-19 updates on its official channel on Telegram. This data is published in a format that is extremely challenging to collect. We rely on the data as collected and made available [on GitHub](https://github.com/idandrd/israel-covid19-data/blob/master/Corona-Tests.csv).
 On 19 April 2020, the person who maintains the GitHub repository confirmed to us that the units refer to the number of tests performed, after checking the information with the Ministry of Health.
 No further information on the geographical scope, number of labs, or types of test included are known.</t>
   </si>
@@ -924,7 +924,7 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000627634.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000628672.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Implementation status of PCR tests for new coronavirus in Japan (based on the date on which the results were determined). Preliminary data</t>
@@ -958,7 +958,7 @@
     <t xml:space="preserve">Kenya - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.go.ke/wp-content/uploads/2020/05/CamScanner-05-05-2020-15.48.16.pdf</t>
+    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1259109013435940866</t>
   </si>
   <si>
     <t xml:space="preserve">Kenya Ministry of Health</t>
@@ -999,7 +999,7 @@
     <t xml:space="preserve">Lithuania - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506175614/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510104952/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
   </si>
   <si>
     <t xml:space="preserve">http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
@@ -1015,7 +1015,7 @@
     <t xml:space="preserve">Luxembourg - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506175621/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200509164113/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
   </si>
   <si>
     <t xml:space="preserve">Luxembourg Government situation update</t>
@@ -1036,7 +1036,7 @@
     <t xml:space="preserve">Malaysia - cases tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506175630/https://www.moh.gov.my/index.php/pages/view/2019-ncov-wuhan</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510105003/https://www.moh.gov.my/index.php/pages/view/2019-ncov-wuhan</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1145,10 +1145,10 @@
     <t xml:space="preserve">Netherlands - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-05/COVID-19_WebSite_rapport_20200506_1112.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 6 May 2020 update</t>
+    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-05/COVID-19_WebSite_rapport_20200509_1018.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 9 May 2020 update</t>
   </si>
   <si>
     <t xml:space="preserve">Dutch National Institute for Public Health and the Environment</t>
@@ -1184,7 +1184,7 @@
     <t xml:space="preserve">Nigeria - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506175710/https://covid19.ncdc.gov.ng/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200508200455/https://covid19.ncdc.gov.ng/</t>
   </si>
   <si>
     <t xml:space="preserve">Nigeria Centre for Disease Control</t>
@@ -1204,7 +1204,7 @@
     <t xml:space="preserve">Norway - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.fhi.no/contentassets/ca5914bd0aa14e15a17f8a7d48fa306a/2020.05.06-dagsrapport-norge-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.fhi.no/contentassets/ca5914bd0aa14e15a17f8a7d48fa306a/2020.05.08-dagsrapport-norge-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Norwegian Institute of Public Health</t>
@@ -1229,7 +1229,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506180000/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510105025/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1259,7 +1259,7 @@
   <si>
     <t xml:space="preserve">The [Panama Ministry of Health](http://www.minsa.gob.pa) in collaboration with the [Gorgas Memorial Institute for Health Studies](http://www.gorgas.gob.pa) reports the cumulative number of tests performed to date in [this dashboard](http://minsa.gob.pa/coronavirus-covid-19). The reported figures include the total number of positive, negative, and "positive control" test results to date.
 It is unclear whether the total number of tests performed ("pruebas realizadas") refers to the number of people tested or the number of samples tested. The number of reported positive test results is equal to the number of confirmed cases of COVID-19, which suggests that the number of tests performed is equivalent to the number of people tested. However, because the data source does not provide a clear definition, we record the units as "unclear".
-Unfortunately, the Ministry of Health's official dashboard does not provide a time series of the number of tests performed each day since testing began. Instead, the dashboard only displays a daily snapshot of the total number of tests performed to date. Since we did not begin to monitor this dashboard until April 14th 2020, we construct a time series dating back to March 9th 2020 using data provided in [this unofficial Github repository](https://github.com/c0t088/DAP-Panama/blob/master/data_covid_pma_dia.csv), which we have cross-referenced against data in the official Ministry of Health dashboard for a sample of dates.</t>
+Unfortunately, the Ministry of Health's official dashboard does not provide a time series of the number of tests performed each day since testing began. Instead, the dashboard only displays a daily snapshot of the total number of tests performed to date. Since we did not begin to monitor this dashboard until April 14th 2020, we construct a time series dating back to March 9th 2020 using data provided in [this unofficial GitHub repository](https://github.com/c0t088/DAP-Panama/blob/master/data_covid_pma_dia.csv), which we have cross-referenced against data in the official Ministry of Health dashboard for a sample of dates.</t>
   </si>
   <si>
     <t xml:space="preserve">PRY</t>
@@ -1284,7 +1284,7 @@
   </si>
   <si>
     <t xml:space="preserve">The Paraguay Ministry of Public Health and Social Welfare provides press releases of the daily number of samples tested, alongside the number of these samples that tested positive. It is unclear whether these figures include samples for which the results are still pending.
-We construct a time series of the daily number of samples tested using the data stored in [this unofficial Github repository](https://github.com/torresmateo/covidpy-rest). We have cross-checked a sample of the figures reported in this unofficial source against the data reported in official press releases.
+We construct a time series of the daily number of samples tested using the data stored in [this unofficial GitHub repository](https://github.com/torresmateo/covidpy-rest). We have cross-checked a sample of the figures reported in this unofficial source against the data reported in official press releases.
 It is possible that the figures are equivalent to the number of people tested, since the number of positive samples reported tend to be equal to the daily number of confirmed cases that the ministry reports. However, since the ministry uses the language "samples taken" ("muestras tomadas") in its press releases, we interpret the units as "sample tested" rather than "people tested".
 The reported figures are cumulative from March 7th 2020, when the first case in Paraguay was confirmed.</t>
   </si>
@@ -1295,7 +1295,7 @@
     <t xml:space="preserve">Peru - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/147296-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-51-189-en-el-peru-comunicado-n-88</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/151163-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-65-015-en-el-peru-comunicado-n-95</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1336,7 +1336,7 @@
     <t xml:space="preserve">Poland - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://raw.githubusercontent.com/anuszka/COVID-19-MZ_GOV_PL/master/data/cor.2020.05.06.csv</t>
+    <t xml:space="preserve">https://raw.githubusercontent.com/anuszka/COVID-19-MZ_GOV_PL/master/data/cor.2020.05.09.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1381,7 +1381,7 @@
     <t xml:space="preserve">Qatar - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506180008/https://www.moph.gov.qa/english/Pages/Coronavirus2019.aspx</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510105040/https://www.moph.gov.qa/english/Pages/Coronavirus2019.aspx</t>
   </si>
   <si>
     <t xml:space="preserve">Qatar Ministry of Public Health</t>
@@ -1409,7 +1409,7 @@
     <t xml:space="preserve">Made available by Adrian-Tudor Panescu on Github</t>
   </si>
   <si>
-    <t xml:space="preserve">Data is collected and made available [on Github](https://github.com/adrianp/covid19romania). It includes a cumulative total of tests performed. No information is given on the geographical scope and number of labs included.
+    <t xml:space="preserve">Data is collected and made available [on GitHub](https://github.com/adrianp/covid19romania). It includes a cumulative total of tests performed. No information is given on the geographical scope and number of labs included.
 The main data source is the press office of the Ministry of Internal Affairs, which provides a daily report on most metrics. Data points are also sourced from the Romanian Ministry of Health and the Romanian National Institute of Public Health and occasionally from news outlets.</t>
   </si>
   <si>
@@ -1419,7 +1419,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14386</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14424</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1439,7 +1439,7 @@
     <t xml:space="preserve">Rwanda - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1257748545744113665</t>
+    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1259173285348204546</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda Ministry of Health</t>
@@ -1512,7 +1512,7 @@
     <t xml:space="preserve">https://www.zdravlje.gov.rs/sekcija/345852/covid-19.php</t>
   </si>
   <si>
-    <t xml:space="preserve">Reports are published daily by the Serbian Ministry of Health. The data is collected and aggregated by volunteers and [published on Github](https://github.com/aleksandar-jovicic/COVID19-Serbia). All labs in Serbia are included.</t>
+    <t xml:space="preserve">Reports are published daily by the Serbian Ministry of Health. The data is collected and aggregated by volunteers and [published on GitHub](https://github.com/aleksandar-jovicic/COVID19-Serbia). All labs in Serbia are included.</t>
   </si>
   <si>
     <t xml:space="preserve">SGP</t>
@@ -1546,7 +1546,7 @@
     <t xml:space="preserve">Slovakia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506180204/https://korona.gov.sk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510105056/https://korona.gov.sk/</t>
   </si>
   <si>
     <t xml:space="preserve">National Center of Health Information and the Office of the Government of the Slovak Republic</t>
@@ -1620,7 +1620,7 @@
     <t xml:space="preserve">South Korea - cases tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367092&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367186&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1640,10 +1640,13 @@
     <t xml:space="preserve">Spain - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/sanidadgob/status/1256993737340747782</t>
+    <t xml:space="preserve">https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov-China/documentos/COVID-19_pruebas_diagnosticas_07_05_2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Consumption and Social Welfare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corresponding press release: https://www.mscbs.gob.es/gabinete/notasPrensa.do?id=4910</t>
   </si>
   <si>
     <t xml:space="preserve">Ministerio de Sanidad, Consumo y Bienestar Social</t>
@@ -1687,9 +1690,6 @@
     <t xml:space="preserve">https://covid-19-schweiz.bagapps.ch/de-3.html</t>
   </si>
   <si>
-    <t xml:space="preserve">BAG dashboard</t>
-  </si>
-  <si>
     <t xml:space="preserve">Federal Office of Public Health</t>
   </si>
   <si>
@@ -1706,7 +1706,7 @@
     <t xml:space="preserve">Taiwan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/DZSBM654J3t3R35Rsh8KJA?typeid=9</t>
+    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/EKvIxtZ0OwCUzeHXum1VBA?typeid=9</t>
   </si>
   <si>
     <t xml:space="preserve">Taiwan Centers for Disease Control (CDC)</t>
@@ -1729,7 +1729,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506180226/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510105142/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1776,7 +1776,7 @@
     <t xml:space="preserve">Turkey - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506180231/https://covid19.saglik.gov.tr/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200509164243/https://covid19.saglik.gov.tr/</t>
   </si>
   <si>
     <t xml:space="preserve">Turkish Ministry of Health</t>
@@ -1800,7 +1800,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1257775905147105280</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1259006502502834181</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
@@ -1823,7 +1823,7 @@
     <t xml:space="preserve">Ukraine - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506180233/https://covid19.gov.ua/en</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510105147/https://covid19.gov.ua/en</t>
   </si>
   <si>
     <t xml:space="preserve">Cabinet of Ministers of Ukraine</t>
@@ -1845,7 +1845,7 @@
     <t xml:space="preserve">United Kingdom - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506180236/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200509164248/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
   </si>
   <si>
     <t xml:space="preserve">Public Health England/Department of Health and Social Care</t>
@@ -1868,7 +1868,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506180240/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200509164249/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
   </si>
   <si>
     <t xml:space="preserve">The number of tests performed, including tests posted or delivered but not yet returned and/or processed.</t>
@@ -1942,7 +1942,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-16</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-20</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -1981,7 +1981,7 @@
     <t xml:space="preserve">Zimbabwe - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1257805665143226377</t>
+    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1258995561090502657</t>
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe Ministry of Health and Child Care</t>
@@ -1991,7 +1991,8 @@
   </si>
   <si>
     <t xml:space="preserve">The Zimbabwe Ministry of Health and Child Care provides daily press releases on its website and Twitter account ([@MoHCCZim](https://twitter.com/MoHCCZim)) that report the cumulative number of tests performed to date. The reported figures include positive, negative, and pending test results. It is not clear how many people have been tested, since the reported figures refer only to the number of tests conducted rather than the number of people tested.
-The earliest reported figure that we have been able to find is from March 15th 2020, at which point 14 tests had been conducted.</t>
+The press release for May 6th 2020 reported that 7,808 PCR and 8,244 "rapid screening" tests had been conducted to date. We exclude rapid screening tests from the daily time series that we construct, since we assume that these are antibody tests.
+Prior to May 6th 2020, the press releases either: (a) reported a combined cumulative total of PCR and rapid screening tests without providing a breakdown between the two types of tests; or (b) did not clearly specify whether the reported cumulative total was in reference to PCR tests, antibody tests, or both. For this reason, the daily time series we construct begins on May 6th 2020, at which point the press releases began to clearly indicate that the reported cumulative totals only include PCR tests.</t>
   </si>
 </sst>
 </file>
@@ -2396,7 +2397,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>43952</v>
+        <v>43960</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -2406,20 +2407,32 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H2" t="n">
-        <v>58685</v>
+        <v>80729</v>
       </c>
       <c r="I2" t="n">
-        <v>1.298</v>
-      </c>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
-      <c r="O2"/>
+        <v>1.786</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2828</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.063</v>
+      </c>
+      <c r="L2" t="n">
+        <v>2804.667</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.062</v>
+      </c>
+      <c r="N2" t="n">
+        <v>2409</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.053</v>
+      </c>
       <c r="P2" t="s">
         <v>22</v>
       </c>
@@ -2441,7 +2454,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
@@ -2451,31 +2464,31 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H3" t="n">
-        <v>688656</v>
+        <v>795456</v>
       </c>
       <c r="I3" t="n">
-        <v>27.006</v>
+        <v>31.194</v>
       </c>
       <c r="J3" t="n">
-        <v>23900</v>
+        <v>38206</v>
       </c>
       <c r="K3" t="n">
-        <v>0.937</v>
+        <v>1.498</v>
       </c>
       <c r="L3" t="n">
-        <v>18516.333</v>
+        <v>35600</v>
       </c>
       <c r="M3" t="n">
-        <v>0.726</v>
+        <v>1.396</v>
       </c>
       <c r="N3" t="n">
-        <v>20606.571</v>
+        <v>26267.571</v>
       </c>
       <c r="O3" t="n">
-        <v>0.808</v>
+        <v>1.03</v>
       </c>
       <c r="P3" t="s">
         <v>29</v>
@@ -2498,7 +2511,7 @@
         <v>33</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>43957</v>
+        <v>43961</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
@@ -2508,31 +2521,31 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="H4" t="n">
-        <v>292254</v>
+        <v>316508</v>
       </c>
       <c r="I4" t="n">
-        <v>32.45</v>
+        <v>35.143</v>
       </c>
       <c r="J4" t="n">
-        <v>6371</v>
+        <v>4818</v>
       </c>
       <c r="K4" t="n">
-        <v>0.707</v>
+        <v>0.535</v>
       </c>
       <c r="L4" t="n">
-        <v>5966.333</v>
+        <v>6204.667</v>
       </c>
       <c r="M4" t="n">
-        <v>0.662</v>
+        <v>0.689</v>
       </c>
       <c r="N4" t="n">
-        <v>6357.143</v>
+        <v>6021.857</v>
       </c>
       <c r="O4" t="n">
-        <v>0.706</v>
+        <v>0.669</v>
       </c>
       <c r="P4" t="s">
         <v>36</v>
@@ -2555,7 +2568,7 @@
         <v>41</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D5" t="s">
         <v>42</v>
@@ -2565,31 +2578,31 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H5" t="n">
-        <v>160341</v>
+        <v>178353</v>
       </c>
       <c r="I5" t="n">
-        <v>94.23</v>
+        <v>104.816</v>
       </c>
       <c r="J5" t="n">
-        <v>4840</v>
+        <v>6195</v>
       </c>
       <c r="K5" t="n">
-        <v>2.844</v>
+        <v>3.641</v>
       </c>
       <c r="L5" t="n">
-        <v>5395.333</v>
+        <v>6004</v>
       </c>
       <c r="M5" t="n">
-        <v>3.171</v>
+        <v>3.529</v>
       </c>
       <c r="N5" t="n">
-        <v>4776.571</v>
+        <v>5725</v>
       </c>
       <c r="O5" t="n">
-        <v>2.807</v>
+        <v>3.365</v>
       </c>
       <c r="P5" t="s">
         <v>44</v>
@@ -2612,7 +2625,7 @@
         <v>49</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D6" t="s">
         <v>50</v>
@@ -2622,31 +2635,31 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H6" t="n">
-        <v>99644</v>
+        <v>116919</v>
       </c>
       <c r="I6" t="n">
-        <v>0.605</v>
+        <v>0.71</v>
       </c>
       <c r="J6" t="n">
-        <v>6241</v>
+        <v>5465</v>
       </c>
       <c r="K6" t="n">
-        <v>0.038</v>
+        <v>0.033</v>
       </c>
       <c r="L6" t="n">
-        <v>6063.333</v>
+        <v>5758.333</v>
       </c>
       <c r="M6" t="n">
-        <v>0.037</v>
+        <v>0.035</v>
       </c>
       <c r="N6" t="n">
-        <v>5706.143</v>
+        <v>5836.143</v>
       </c>
       <c r="O6" t="n">
-        <v>0.035</v>
+        <v>0.036</v>
       </c>
       <c r="P6" t="s">
         <v>51</v>
@@ -2669,7 +2682,7 @@
         <v>56</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>43955</v>
+        <v>43959</v>
       </c>
       <c r="D7" t="s">
         <v>57</v>
@@ -2679,16 +2692,20 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H7" t="n">
-        <v>211369</v>
+        <v>240146</v>
       </c>
       <c r="I7" t="n">
-        <v>22.369</v>
-      </c>
-      <c r="J7"/>
-      <c r="K7"/>
+        <v>25.414</v>
+      </c>
+      <c r="J7" t="n">
+        <v>10680</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1.13</v>
+      </c>
       <c r="L7"/>
       <c r="M7"/>
       <c r="N7"/>
@@ -2714,7 +2731,7 @@
         <v>62</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>43955</v>
+        <v>43959</v>
       </c>
       <c r="D8" t="s">
         <v>63</v>
@@ -2724,31 +2741,31 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="H8" t="n">
-        <v>391314</v>
+        <v>461303</v>
       </c>
       <c r="I8" t="n">
-        <v>33.764</v>
+        <v>39.803</v>
       </c>
       <c r="J8" t="n">
-        <v>19721</v>
+        <v>21311</v>
       </c>
       <c r="K8" t="n">
-        <v>1.702</v>
+        <v>1.839</v>
       </c>
       <c r="L8" t="n">
-        <v>15552.667</v>
+        <v>18816.667</v>
       </c>
       <c r="M8" t="n">
-        <v>1.342</v>
+        <v>1.624</v>
       </c>
       <c r="N8" t="n">
-        <v>18086.286</v>
+        <v>17504.143</v>
       </c>
       <c r="O8" t="n">
-        <v>1.561</v>
+        <v>1.51</v>
       </c>
       <c r="P8" t="s">
         <v>64</v>
@@ -2771,7 +2788,7 @@
         <v>69</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D9" t="s">
         <v>70</v>
@@ -2783,31 +2800,31 @@
         <v>71</v>
       </c>
       <c r="G9" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H9" t="n">
-        <v>7888</v>
+        <v>8523</v>
       </c>
       <c r="I9" t="n">
-        <v>0.676</v>
+        <v>0.73</v>
       </c>
       <c r="J9" t="n">
-        <v>121</v>
+        <v>171</v>
       </c>
       <c r="K9" t="n">
-        <v>0.01</v>
+        <v>0.015</v>
       </c>
       <c r="L9" t="n">
-        <v>110.667</v>
+        <v>183.667</v>
       </c>
       <c r="M9" t="n">
-        <v>0.009</v>
+        <v>0.016</v>
       </c>
       <c r="N9" t="n">
-        <v>252.429</v>
+        <v>138.143</v>
       </c>
       <c r="O9" t="n">
-        <v>0.022</v>
+        <v>0.012</v>
       </c>
       <c r="P9" t="s">
         <v>43</v>
@@ -2875,7 +2892,7 @@
         <v>83</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>43957</v>
+        <v>43961</v>
       </c>
       <c r="D11" t="s">
         <v>84</v>
@@ -2885,28 +2902,32 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H11" t="n">
-        <v>51768</v>
+        <v>57231</v>
       </c>
       <c r="I11" t="n">
-        <v>7.45</v>
+        <v>8.237</v>
       </c>
       <c r="J11" t="n">
-        <v>1465</v>
+        <v>1126</v>
       </c>
       <c r="K11" t="n">
-        <v>0.211</v>
+        <v>0.162</v>
       </c>
       <c r="L11" t="n">
-        <v>1050</v>
+        <v>1433.333</v>
       </c>
       <c r="M11" t="n">
-        <v>0.151</v>
-      </c>
-      <c r="N11"/>
-      <c r="O11"/>
+        <v>0.206</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1230.429</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.177</v>
+      </c>
       <c r="P11" t="s">
         <v>86</v>
       </c>
@@ -2928,7 +2949,7 @@
         <v>90</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>43957</v>
+        <v>43961</v>
       </c>
       <c r="D12" t="s">
         <v>91</v>
@@ -2938,24 +2959,26 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H12" t="n">
-        <v>942526</v>
+        <v>1071379</v>
       </c>
       <c r="I12" t="n">
-        <v>24.973</v>
+        <v>28.387</v>
       </c>
       <c r="J12"/>
       <c r="K12" t="n">
-        <v>0.052</v>
+        <v>0.1</v>
       </c>
       <c r="L12"/>
       <c r="M12" t="n">
-        <v>0.433</v>
+        <v>0.614</v>
       </c>
       <c r="N12"/>
-      <c r="O12"/>
+      <c r="O12" t="n">
+        <v>0.673</v>
+      </c>
       <c r="P12" t="s">
         <v>92</v>
       </c>
@@ -2977,7 +3000,7 @@
         <v>97</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D13" t="s">
         <v>98</v>
@@ -2989,31 +3012,31 @@
         <v>99</v>
       </c>
       <c r="G13" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H13" t="n">
-        <v>232108</v>
+        <v>267904</v>
       </c>
       <c r="I13" t="n">
-        <v>12.142</v>
+        <v>14.014</v>
       </c>
       <c r="J13" t="n">
-        <v>10013</v>
+        <v>11943</v>
       </c>
       <c r="K13" t="n">
-        <v>0.524</v>
+        <v>0.625</v>
       </c>
       <c r="L13" t="n">
-        <v>8630</v>
+        <v>11932</v>
       </c>
       <c r="M13" t="n">
-        <v>0.452</v>
+        <v>0.624</v>
       </c>
       <c r="N13" t="n">
-        <v>8498.429</v>
+        <v>9786.286</v>
       </c>
       <c r="O13" t="n">
-        <v>0.445</v>
+        <v>0.512</v>
       </c>
       <c r="P13" t="s">
         <v>100</v>
@@ -3036,7 +3059,7 @@
         <v>104</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D14" t="s">
         <v>105</v>
@@ -3046,31 +3069,31 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H14" t="n">
-        <v>127105</v>
+        <v>144912</v>
       </c>
       <c r="I14" t="n">
-        <v>2.498</v>
+        <v>2.848</v>
       </c>
       <c r="J14" t="n">
-        <v>4076</v>
+        <v>5173</v>
       </c>
       <c r="K14" t="n">
-        <v>0.08</v>
+        <v>0.102</v>
       </c>
       <c r="L14" t="n">
-        <v>4167.667</v>
+        <v>4600.667</v>
       </c>
       <c r="M14" t="n">
-        <v>0.082</v>
+        <v>0.09</v>
       </c>
       <c r="N14" t="n">
-        <v>4574.286</v>
+        <v>4330</v>
       </c>
       <c r="O14" t="n">
-        <v>0.09</v>
+        <v>0.085</v>
       </c>
       <c r="P14" t="s">
         <v>106</v>
@@ -3093,7 +3116,7 @@
         <v>111</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D15" t="s">
         <v>112</v>
@@ -3103,31 +3126,31 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H15" t="n">
-        <v>9892</v>
+        <v>11276</v>
       </c>
       <c r="I15" t="n">
-        <v>1.942</v>
+        <v>2.214</v>
       </c>
       <c r="J15" t="n">
-        <v>73</v>
+        <v>449</v>
       </c>
       <c r="K15" t="n">
-        <v>0.014</v>
+        <v>0.088</v>
       </c>
       <c r="L15" t="n">
-        <v>99.667</v>
+        <v>391.667</v>
       </c>
       <c r="M15" t="n">
-        <v>0.02</v>
+        <v>0.077</v>
       </c>
       <c r="N15" t="n">
-        <v>129</v>
+        <v>240.429</v>
       </c>
       <c r="O15" t="n">
-        <v>0.025</v>
+        <v>0.047</v>
       </c>
       <c r="P15" t="s">
         <v>113</v>
@@ -3150,7 +3173,7 @@
         <v>117</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D16" t="s">
         <v>118</v>
@@ -3160,28 +3183,32 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H16" t="n">
-        <v>41053</v>
+        <v>44218</v>
       </c>
       <c r="I16" t="n">
-        <v>10</v>
+        <v>10.771</v>
       </c>
       <c r="J16" t="n">
-        <v>1080</v>
+        <v>840</v>
       </c>
       <c r="K16" t="n">
-        <v>0.263</v>
+        <v>0.205</v>
       </c>
       <c r="L16" t="n">
-        <v>989.667</v>
+        <v>1055</v>
       </c>
       <c r="M16" t="n">
-        <v>0.241</v>
-      </c>
-      <c r="N16"/>
-      <c r="O16"/>
+        <v>0.257</v>
+      </c>
+      <c r="N16" t="n">
+        <v>951.571</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.232</v>
+      </c>
       <c r="P16" t="s">
         <v>119</v>
       </c>
@@ -3203,7 +3230,7 @@
         <v>124</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>43956</v>
+        <v>43959</v>
       </c>
       <c r="D17" t="s">
         <v>125</v>
@@ -3215,31 +3242,31 @@
         <v>127</v>
       </c>
       <c r="G17" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H17" t="n">
-        <v>59648</v>
+        <v>65509</v>
       </c>
       <c r="I17" t="n">
-        <v>5.266</v>
+        <v>5.784</v>
       </c>
       <c r="J17" t="n">
-        <v>1937</v>
+        <v>1949</v>
       </c>
       <c r="K17" t="n">
-        <v>0.171</v>
+        <v>0.172</v>
       </c>
       <c r="L17" t="n">
-        <v>2034.333</v>
+        <v>1953.667</v>
       </c>
       <c r="M17" t="n">
-        <v>0.179</v>
+        <v>0.172</v>
       </c>
       <c r="N17" t="n">
-        <v>2043.429</v>
+        <v>2000.429</v>
       </c>
       <c r="O17" t="n">
-        <v>0.18</v>
+        <v>0.176</v>
       </c>
       <c r="P17" t="s">
         <v>126</v>
@@ -3262,7 +3289,7 @@
         <v>131</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D18" t="s">
         <v>132</v>
@@ -3272,31 +3299,31 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="H18" t="n">
-        <v>278519</v>
+        <v>302493</v>
       </c>
       <c r="I18" t="n">
-        <v>26.008</v>
+        <v>28.247</v>
       </c>
       <c r="J18" t="n">
-        <v>9416</v>
+        <v>3717</v>
       </c>
       <c r="K18" t="n">
-        <v>0.879</v>
+        <v>0.347</v>
       </c>
       <c r="L18" t="n">
-        <v>6879.333</v>
+        <v>5193.333</v>
       </c>
       <c r="M18" t="n">
-        <v>0.642</v>
+        <v>0.485</v>
       </c>
       <c r="N18" t="n">
-        <v>6207.714</v>
+        <v>6373.143</v>
       </c>
       <c r="O18" t="n">
-        <v>0.58</v>
+        <v>0.595</v>
       </c>
       <c r="P18" t="s">
         <v>43</v>
@@ -3319,7 +3346,7 @@
         <v>136</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D19" t="s">
         <v>137</v>
@@ -3331,31 +3358,31 @@
         <v>139</v>
       </c>
       <c r="G19" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H19" t="n">
-        <v>270680</v>
+        <v>308984</v>
       </c>
       <c r="I19" t="n">
-        <v>46.732</v>
+        <v>53.345</v>
       </c>
       <c r="J19" t="n">
-        <v>12942</v>
+        <v>10496</v>
       </c>
       <c r="K19" t="n">
-        <v>2.234</v>
+        <v>1.812</v>
       </c>
       <c r="L19" t="n">
-        <v>12293.667</v>
+        <v>12768</v>
       </c>
       <c r="M19" t="n">
-        <v>2.122</v>
+        <v>2.204</v>
       </c>
       <c r="N19" t="n">
-        <v>12945.429</v>
+        <v>12438.857</v>
       </c>
       <c r="O19" t="n">
-        <v>2.235</v>
+        <v>2.147</v>
       </c>
       <c r="P19" t="s">
         <v>140</v>
@@ -3378,7 +3405,7 @@
         <v>144</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>43955</v>
+        <v>43959</v>
       </c>
       <c r="D20" t="s">
         <v>145</v>
@@ -3390,26 +3417,22 @@
         <v>147</v>
       </c>
       <c r="G20" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H20" t="n">
-        <v>66160</v>
+        <v>40630</v>
       </c>
       <c r="I20" t="n">
-        <v>3.75</v>
+        <v>2.303</v>
       </c>
       <c r="J20"/>
       <c r="K20" t="n">
-        <v>0.211</v>
+        <v>-0.212</v>
       </c>
       <c r="L20"/>
-      <c r="M20" t="n">
-        <v>0.55</v>
-      </c>
+      <c r="M20"/>
       <c r="N20"/>
-      <c r="O20" t="n">
-        <v>0.284</v>
-      </c>
+      <c r="O20"/>
       <c r="P20" t="s">
         <v>146</v>
       </c>
@@ -3431,7 +3454,7 @@
         <v>151</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D21" t="s">
         <v>152</v>
@@ -3443,26 +3466,22 @@
         <v>154</v>
       </c>
       <c r="G21" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H21" t="n">
-        <v>33628</v>
+        <v>39079</v>
       </c>
       <c r="I21" t="n">
-        <v>5.185</v>
+        <v>6.025</v>
       </c>
       <c r="J21" t="n">
-        <v>1598</v>
+        <v>1773</v>
       </c>
       <c r="K21" t="n">
-        <v>0.246</v>
-      </c>
-      <c r="L21" t="n">
-        <v>1677.333</v>
-      </c>
-      <c r="M21" t="n">
-        <v>0.258</v>
-      </c>
+        <v>0.273</v>
+      </c>
+      <c r="L21"/>
+      <c r="M21"/>
       <c r="N21"/>
       <c r="O21"/>
       <c r="P21" t="s">
@@ -3486,7 +3505,7 @@
         <v>157</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D22" t="s">
         <v>158</v>
@@ -3496,31 +3515,31 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="H22" t="n">
-        <v>58955</v>
+        <v>63372</v>
       </c>
       <c r="I22" t="n">
-        <v>44.443</v>
+        <v>47.772</v>
       </c>
       <c r="J22" t="n">
-        <v>1541</v>
+        <v>654</v>
       </c>
       <c r="K22" t="n">
-        <v>1.162</v>
+        <v>0.493</v>
       </c>
       <c r="L22" t="n">
-        <v>1256.667</v>
+        <v>961.333</v>
       </c>
       <c r="M22" t="n">
-        <v>0.947</v>
+        <v>0.725</v>
       </c>
       <c r="N22" t="n">
-        <v>1112.143</v>
+        <v>1170.714</v>
       </c>
       <c r="O22" t="n">
-        <v>0.838</v>
+        <v>0.882</v>
       </c>
       <c r="P22" t="s">
         <v>160</v>
@@ -3543,7 +3562,7 @@
         <v>165</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D23" t="s">
         <v>166</v>
@@ -3553,16 +3572,20 @@
       </c>
       <c r="F23"/>
       <c r="G23" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H23" t="n">
-        <v>26517</v>
+        <v>30306</v>
       </c>
       <c r="I23" t="n">
-        <v>0.231</v>
-      </c>
-      <c r="J23"/>
-      <c r="K23"/>
+        <v>0.264</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1946</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.017</v>
+      </c>
       <c r="L23"/>
       <c r="M23"/>
       <c r="N23"/>
@@ -3588,7 +3611,7 @@
         <v>171</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>43956</v>
+        <v>43959</v>
       </c>
       <c r="D24" t="s">
         <v>172</v>
@@ -3598,25 +3621,25 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H24" t="n">
-        <v>108112</v>
+        <v>119054</v>
       </c>
       <c r="I24" t="n">
-        <v>19.512</v>
+        <v>21.487</v>
       </c>
       <c r="J24"/>
       <c r="K24" t="n">
-        <v>0.098</v>
+        <v>0.116</v>
       </c>
       <c r="L24"/>
       <c r="M24" t="n">
-        <v>0.184</v>
+        <v>0.433</v>
       </c>
       <c r="N24"/>
       <c r="O24" t="n">
-        <v>0.375</v>
+        <v>0.388</v>
       </c>
       <c r="P24" t="s">
         <v>174</v>
@@ -3639,7 +3662,7 @@
         <v>177</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>43949</v>
+        <v>43956</v>
       </c>
       <c r="D25" t="s">
         <v>178</v>
@@ -3651,13 +3674,13 @@
         <v>180</v>
       </c>
       <c r="G25" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H25" t="n">
-        <v>724574</v>
+        <v>831174</v>
       </c>
       <c r="I25" t="n">
-        <v>11.101</v>
+        <v>12.734</v>
       </c>
       <c r="J25"/>
       <c r="K25"/>
@@ -3733,7 +3756,7 @@
         <v>192</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>43953</v>
+        <v>43958</v>
       </c>
       <c r="D27" t="s">
         <v>193</v>
@@ -3743,20 +3766,16 @@
       </c>
       <c r="F27"/>
       <c r="G27" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H27" t="n">
-        <v>129461</v>
+        <v>149948</v>
       </c>
       <c r="I27" t="n">
-        <v>4.166</v>
-      </c>
-      <c r="J27" t="n">
-        <v>12412</v>
-      </c>
-      <c r="K27" t="n">
-        <v>0.399</v>
-      </c>
+        <v>4.826</v>
+      </c>
+      <c r="J27"/>
+      <c r="K27"/>
       <c r="L27"/>
       <c r="M27"/>
       <c r="N27"/>
@@ -3782,7 +3801,7 @@
         <v>200</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D28" t="s">
         <v>201</v>
@@ -3792,18 +3811,26 @@
       </c>
       <c r="F28"/>
       <c r="G28" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H28" t="n">
-        <v>87052</v>
+        <v>97384</v>
       </c>
       <c r="I28" t="n">
-        <v>8.352</v>
-      </c>
-      <c r="J28"/>
-      <c r="K28"/>
-      <c r="L28"/>
-      <c r="M28"/>
+        <v>9.343</v>
+      </c>
+      <c r="J28" t="n">
+        <v>3093</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.297</v>
+      </c>
+      <c r="L28" t="n">
+        <v>3444</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.331</v>
+      </c>
       <c r="N28"/>
       <c r="O28"/>
       <c r="P28" t="s">
@@ -3827,7 +3854,7 @@
         <v>207</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>43948</v>
+        <v>43956</v>
       </c>
       <c r="D29" t="s">
         <v>208</v>
@@ -3837,13 +3864,13 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H29" t="n">
-        <v>154989</v>
+        <v>168291</v>
       </c>
       <c r="I29" t="n">
-        <v>20.674</v>
+        <v>22.448</v>
       </c>
       <c r="J29"/>
       <c r="K29"/>
@@ -3872,7 +3899,7 @@
         <v>214</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>43957</v>
+        <v>43961</v>
       </c>
       <c r="D30" t="s">
         <v>215</v>
@@ -3884,31 +3911,31 @@
         <v>217</v>
       </c>
       <c r="G30" t="n">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H30" t="n">
-        <v>86743</v>
+        <v>108257</v>
       </c>
       <c r="I30" t="n">
-        <v>8.979</v>
+        <v>11.206</v>
       </c>
       <c r="J30" t="n">
-        <v>1186</v>
+        <v>4999</v>
       </c>
       <c r="K30" t="n">
-        <v>0.123</v>
+        <v>0.517</v>
       </c>
       <c r="L30" t="n">
-        <v>1577.667</v>
+        <v>4740.333</v>
       </c>
       <c r="M30" t="n">
-        <v>0.164</v>
+        <v>0.491</v>
       </c>
       <c r="N30" t="n">
-        <v>2349</v>
+        <v>3749.571</v>
       </c>
       <c r="O30" t="n">
-        <v>0.243</v>
+        <v>0.388</v>
       </c>
       <c r="P30" t="s">
         <v>216</v>
@@ -3931,7 +3958,7 @@
         <v>222</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>43956</v>
+        <v>43959</v>
       </c>
       <c r="D31" t="s">
         <v>223</v>
@@ -3941,25 +3968,31 @@
       </c>
       <c r="F31"/>
       <c r="G31" t="n">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H31" t="n">
-        <v>51622</v>
+        <v>53219</v>
       </c>
       <c r="I31" t="n">
-        <v>151.273</v>
-      </c>
-      <c r="J31"/>
+        <v>155.953</v>
+      </c>
+      <c r="J31" t="n">
+        <v>515</v>
+      </c>
       <c r="K31" t="n">
-        <v>0.932</v>
-      </c>
-      <c r="L31"/>
+        <v>1.509</v>
+      </c>
+      <c r="L31" t="n">
+        <v>532.333</v>
+      </c>
       <c r="M31" t="n">
-        <v>1.228</v>
-      </c>
-      <c r="N31"/>
+        <v>1.56</v>
+      </c>
+      <c r="N31" t="n">
+        <v>465.429</v>
+      </c>
       <c r="O31" t="n">
-        <v>1.712</v>
+        <v>1.364</v>
       </c>
       <c r="P31" t="s">
         <v>224</v>
@@ -4033,7 +4066,7 @@
         <v>233</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>43957</v>
+        <v>43961</v>
       </c>
       <c r="D33" t="s">
         <v>229</v>
@@ -4045,31 +4078,31 @@
         <v>231</v>
       </c>
       <c r="G33" t="n">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H33" t="n">
-        <v>1276781</v>
+        <v>1609037</v>
       </c>
       <c r="I33" t="n">
-        <v>0.925</v>
+        <v>1.166</v>
       </c>
       <c r="J33" t="n">
-        <v>84835</v>
+        <v>85824</v>
       </c>
       <c r="K33" t="n">
+        <v>0.062</v>
+      </c>
+      <c r="L33" t="n">
+        <v>83874.667</v>
+      </c>
+      <c r="M33" t="n">
         <v>0.061</v>
       </c>
-      <c r="L33" t="n">
-        <v>76777</v>
-      </c>
-      <c r="M33" t="n">
-        <v>0.055</v>
-      </c>
       <c r="N33" t="n">
-        <v>72288.143</v>
+        <v>80369.571</v>
       </c>
       <c r="O33" t="n">
-        <v>0.052</v>
+        <v>0.058</v>
       </c>
       <c r="P33" t="s">
         <v>230</v>
@@ -4092,7 +4125,7 @@
         <v>235</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>43957</v>
+        <v>43961</v>
       </c>
       <c r="D34" t="s">
         <v>236</v>
@@ -4102,31 +4135,31 @@
       </c>
       <c r="F34"/>
       <c r="G34" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H34" t="n">
-        <v>92976</v>
+        <v>113452</v>
       </c>
       <c r="I34" t="n">
-        <v>0.34</v>
+        <v>0.415</v>
       </c>
       <c r="J34" t="n">
-        <v>4052</v>
+        <v>4753</v>
       </c>
       <c r="K34" t="n">
-        <v>0.015</v>
+        <v>0.017</v>
       </c>
       <c r="L34" t="n">
-        <v>3321.333</v>
+        <v>5578.333</v>
       </c>
       <c r="M34" t="n">
-        <v>0.012</v>
+        <v>0.02</v>
       </c>
       <c r="N34" t="n">
-        <v>3598.857</v>
+        <v>4348.571</v>
       </c>
       <c r="O34" t="n">
-        <v>0.013</v>
+        <v>0.016</v>
       </c>
       <c r="P34" t="s">
         <v>237</v>
@@ -4149,7 +4182,7 @@
         <v>241</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D35" t="s">
         <v>242</v>
@@ -4159,31 +4192,31 @@
       </c>
       <c r="F35"/>
       <c r="G35" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H35" t="n">
-        <v>531275</v>
+        <v>558899</v>
       </c>
       <c r="I35" t="n">
-        <v>6.325</v>
+        <v>6.654</v>
       </c>
       <c r="J35" t="n">
-        <v>11732</v>
+        <v>14107</v>
       </c>
       <c r="K35" t="n">
-        <v>0.14</v>
+        <v>0.168</v>
       </c>
       <c r="L35" t="n">
-        <v>11667.333</v>
+        <v>13118.667</v>
       </c>
       <c r="M35" t="n">
-        <v>0.139</v>
+        <v>0.156</v>
       </c>
       <c r="N35" t="n">
-        <v>11127</v>
+        <v>11982.286</v>
       </c>
       <c r="O35" t="n">
-        <v>0.133</v>
+        <v>0.143</v>
       </c>
       <c r="P35" t="s">
         <v>243</v>
@@ -4251,7 +4284,7 @@
         <v>253</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D37" t="s">
         <v>254</v>
@@ -4263,25 +4296,31 @@
         <v>256</v>
       </c>
       <c r="G37" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H37" t="n">
-        <v>413517</v>
+        <v>435790</v>
       </c>
       <c r="I37" t="n">
-        <v>47.775</v>
-      </c>
-      <c r="J37"/>
+        <v>50.348</v>
+      </c>
+      <c r="J37" t="n">
+        <v>8876</v>
+      </c>
       <c r="K37" t="n">
-        <v>0.302</v>
-      </c>
-      <c r="L37"/>
+        <v>1.025</v>
+      </c>
+      <c r="L37" t="n">
+        <v>9003.333</v>
+      </c>
       <c r="M37" t="n">
-        <v>0.803</v>
-      </c>
-      <c r="N37"/>
+        <v>1.04</v>
+      </c>
+      <c r="N37" t="n">
+        <v>8844</v>
+      </c>
       <c r="O37" t="n">
-        <v>0.968</v>
+        <v>1.022</v>
       </c>
       <c r="P37" t="s">
         <v>43</v>
@@ -4304,7 +4343,7 @@
         <v>260</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D38" t="s">
         <v>261</v>
@@ -4316,31 +4355,31 @@
         <v>263</v>
       </c>
       <c r="G38" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H38" t="n">
-        <v>1549892</v>
+        <v>1645076</v>
       </c>
       <c r="I38" t="n">
-        <v>25.634</v>
+        <v>27.209</v>
       </c>
       <c r="J38" t="n">
-        <v>37771</v>
+        <v>36091</v>
       </c>
       <c r="K38" t="n">
-        <v>0.625</v>
+        <v>0.597</v>
       </c>
       <c r="L38" t="n">
-        <v>30993.667</v>
+        <v>31728</v>
       </c>
       <c r="M38" t="n">
-        <v>0.513</v>
+        <v>0.525</v>
       </c>
       <c r="N38" t="n">
-        <v>33776</v>
+        <v>30744.571</v>
       </c>
       <c r="O38" t="n">
-        <v>0.559</v>
+        <v>0.508</v>
       </c>
       <c r="P38" t="s">
         <v>264</v>
@@ -4363,7 +4402,7 @@
         <v>267</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D39" t="s">
         <v>261</v>
@@ -4375,31 +4414,31 @@
         <v>263</v>
       </c>
       <c r="G39" t="n">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H39" t="n">
-        <v>2310929</v>
+        <v>2514234</v>
       </c>
       <c r="I39" t="n">
-        <v>38.221</v>
+        <v>41.584</v>
       </c>
       <c r="J39" t="n">
-        <v>64263</v>
+        <v>69171</v>
       </c>
       <c r="K39" t="n">
-        <v>1.063</v>
+        <v>1.144</v>
       </c>
       <c r="L39" t="n">
-        <v>52385.667</v>
+        <v>67768.333</v>
       </c>
       <c r="M39" t="n">
-        <v>0.866</v>
+        <v>1.121</v>
       </c>
       <c r="N39" t="n">
-        <v>57166.857</v>
+        <v>57913.857</v>
       </c>
       <c r="O39" t="n">
-        <v>0.945</v>
+        <v>0.958</v>
       </c>
       <c r="P39" t="s">
         <v>264</v>
@@ -4422,7 +4461,7 @@
         <v>270</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D40" t="s">
         <v>271</v>
@@ -4434,13 +4473,13 @@
         <v>273</v>
       </c>
       <c r="G40" t="n">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H40" t="n">
-        <v>188927</v>
+        <v>211997</v>
       </c>
       <c r="I40" t="n">
-        <v>1.494</v>
+        <v>1.676</v>
       </c>
       <c r="J40"/>
       <c r="K40"/>
@@ -4469,7 +4508,7 @@
         <v>276</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>43955</v>
+        <v>43958</v>
       </c>
       <c r="D41" t="s">
         <v>277</v>
@@ -4481,31 +4520,31 @@
         <v>278</v>
       </c>
       <c r="G41" t="n">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="H41" t="n">
-        <v>285356</v>
+        <v>312728</v>
       </c>
       <c r="I41" t="n">
-        <v>2.256</v>
+        <v>2.473</v>
       </c>
       <c r="J41" t="n">
-        <v>2049</v>
+        <v>6061</v>
       </c>
       <c r="K41" t="n">
-        <v>0.016</v>
+        <v>0.048</v>
       </c>
       <c r="L41" t="n">
-        <v>2602.667</v>
+        <v>4768.667</v>
       </c>
       <c r="M41" t="n">
-        <v>0.02</v>
+        <v>0.038</v>
       </c>
       <c r="N41" t="n">
-        <v>4773.857</v>
+        <v>5210.143</v>
       </c>
       <c r="O41" t="n">
-        <v>0.038</v>
+        <v>0.041</v>
       </c>
       <c r="P41" t="s">
         <v>272</v>
@@ -4528,7 +4567,7 @@
         <v>281</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D42" t="s">
         <v>282</v>
@@ -4538,31 +4577,31 @@
       </c>
       <c r="F42"/>
       <c r="G42" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H42" t="n">
-        <v>336480</v>
+        <v>385104</v>
       </c>
       <c r="I42" t="n">
-        <v>17.92</v>
+        <v>20.51</v>
       </c>
       <c r="J42" t="n">
-        <v>16069</v>
+        <v>13978</v>
       </c>
       <c r="K42" t="n">
-        <v>0.856</v>
+        <v>0.744</v>
       </c>
       <c r="L42" t="n">
-        <v>13448</v>
+        <v>16208</v>
       </c>
       <c r="M42" t="n">
-        <v>0.716</v>
+        <v>0.863</v>
       </c>
       <c r="N42" t="n">
-        <v>14866.429</v>
+        <v>14606</v>
       </c>
       <c r="O42" t="n">
-        <v>0.792</v>
+        <v>0.778</v>
       </c>
       <c r="P42" t="s">
         <v>283</v>
@@ -4585,7 +4624,7 @@
         <v>286</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D43" t="s">
         <v>287</v>
@@ -4595,26 +4634,22 @@
       </c>
       <c r="F43"/>
       <c r="G43" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H43" t="n">
-        <v>25869</v>
+        <v>31041</v>
       </c>
       <c r="I43" t="n">
-        <v>0.481</v>
+        <v>0.577</v>
       </c>
       <c r="J43" t="n">
-        <v>1077</v>
+        <v>1611</v>
       </c>
       <c r="K43" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="L43" t="n">
-        <v>990.667</v>
-      </c>
-      <c r="M43" t="n">
-        <v>0.018</v>
-      </c>
+        <v>0.03</v>
+      </c>
+      <c r="L43"/>
+      <c r="M43"/>
       <c r="N43"/>
       <c r="O43"/>
       <c r="P43" t="s">
@@ -4638,7 +4673,7 @@
         <v>293</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>43957</v>
+        <v>43961</v>
       </c>
       <c r="D44" t="s">
         <v>294</v>
@@ -4650,31 +4685,25 @@
         <v>296</v>
       </c>
       <c r="G44" t="n">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="H44" t="n">
-        <v>68627</v>
+        <v>76592</v>
       </c>
       <c r="I44" t="n">
-        <v>36.384</v>
-      </c>
-      <c r="J44" t="n">
-        <v>2477</v>
-      </c>
+        <v>40.606</v>
+      </c>
+      <c r="J44"/>
       <c r="K44" t="n">
-        <v>1.313</v>
-      </c>
-      <c r="L44" t="n">
-        <v>1460.667</v>
-      </c>
+        <v>0.541</v>
+      </c>
+      <c r="L44"/>
       <c r="M44" t="n">
-        <v>0.774</v>
-      </c>
-      <c r="N44" t="n">
-        <v>1973.714</v>
-      </c>
+        <v>0.976</v>
+      </c>
+      <c r="N44"/>
       <c r="O44" t="n">
-        <v>1.046</v>
+        <v>0.935</v>
       </c>
       <c r="P44" t="s">
         <v>295</v>
@@ -4697,7 +4726,7 @@
         <v>299</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>43957</v>
+        <v>43961</v>
       </c>
       <c r="D45" t="s">
         <v>300</v>
@@ -4707,31 +4736,25 @@
       </c>
       <c r="F45"/>
       <c r="G45" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H45" t="n">
-        <v>156493</v>
+        <v>183913</v>
       </c>
       <c r="I45" t="n">
-        <v>57.486</v>
-      </c>
-      <c r="J45" t="n">
-        <v>7387</v>
-      </c>
+        <v>67.558</v>
+      </c>
+      <c r="J45"/>
       <c r="K45" t="n">
-        <v>2.714</v>
-      </c>
-      <c r="L45" t="n">
-        <v>4938.333</v>
-      </c>
+        <v>1.315</v>
+      </c>
+      <c r="L45"/>
       <c r="M45" t="n">
-        <v>1.814</v>
-      </c>
-      <c r="N45" t="n">
-        <v>5470.286</v>
-      </c>
+        <v>2.427</v>
+      </c>
+      <c r="N45"/>
       <c r="O45" t="n">
-        <v>2.01</v>
+        <v>2.216</v>
       </c>
       <c r="P45" t="s">
         <v>43</v>
@@ -4754,7 +4777,7 @@
         <v>304</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D46" t="s">
         <v>305</v>
@@ -4764,31 +4787,31 @@
       </c>
       <c r="F46"/>
       <c r="G46" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H46" t="n">
-        <v>50533</v>
+        <v>54463</v>
       </c>
       <c r="I46" t="n">
-        <v>80.727</v>
+        <v>87.005</v>
       </c>
       <c r="J46" t="n">
-        <v>1234</v>
+        <v>1206</v>
       </c>
       <c r="K46" t="n">
-        <v>1.971</v>
+        <v>1.927</v>
       </c>
       <c r="L46" t="n">
-        <v>805</v>
+        <v>1310</v>
       </c>
       <c r="M46" t="n">
-        <v>1.286</v>
+        <v>2.093</v>
       </c>
       <c r="N46" t="n">
-        <v>1253.571</v>
+        <v>1000.429</v>
       </c>
       <c r="O46" t="n">
-        <v>2.003</v>
+        <v>1.598</v>
       </c>
       <c r="P46" t="s">
         <v>306</v>
@@ -4811,7 +4834,7 @@
         <v>310</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>43957</v>
+        <v>43961</v>
       </c>
       <c r="D47" t="s">
         <v>311</v>
@@ -4821,26 +4844,18 @@
       </c>
       <c r="F47"/>
       <c r="G47" t="n">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H47" t="n">
-        <v>222150</v>
+        <v>256937</v>
       </c>
       <c r="I47" t="n">
-        <v>6.864</v>
-      </c>
-      <c r="J47" t="n">
-        <v>8930</v>
-      </c>
-      <c r="K47" t="n">
-        <v>0.276</v>
-      </c>
-      <c r="L47" t="n">
-        <v>8772.333</v>
-      </c>
-      <c r="M47" t="n">
-        <v>0.271</v>
-      </c>
+        <v>7.938</v>
+      </c>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
       <c r="N47"/>
       <c r="O47"/>
       <c r="P47" t="s">
@@ -4864,7 +4879,7 @@
         <v>317</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D48" t="s">
         <v>318</v>
@@ -4874,13 +4889,13 @@
       </c>
       <c r="F48"/>
       <c r="G48" t="n">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="H48" t="n">
-        <v>89565</v>
+        <v>107261</v>
       </c>
       <c r="I48" t="n">
-        <v>0.695</v>
+        <v>0.832</v>
       </c>
       <c r="J48"/>
       <c r="K48" t="n">
@@ -4888,11 +4903,11 @@
       </c>
       <c r="L48"/>
       <c r="M48" t="n">
-        <v>0.002</v>
+        <v>0.004</v>
       </c>
       <c r="N48"/>
       <c r="O48" t="n">
-        <v>0.011</v>
+        <v>0.014</v>
       </c>
       <c r="P48" t="s">
         <v>319</v>
@@ -4974,7 +4989,7 @@
         <v>329</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D50" t="s">
         <v>330</v>
@@ -4986,20 +5001,32 @@
         <v>332</v>
       </c>
       <c r="G50" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H50" t="n">
-        <v>9295</v>
+        <v>10848</v>
       </c>
       <c r="I50" t="n">
-        <v>0.171</v>
-      </c>
-      <c r="J50"/>
-      <c r="K50"/>
-      <c r="L50"/>
-      <c r="M50"/>
-      <c r="N50"/>
-      <c r="O50"/>
+        <v>0.199</v>
+      </c>
+      <c r="J50" t="n">
+        <v>582</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="L50" t="n">
+        <v>517.667</v>
+      </c>
+      <c r="M50" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="N50" t="n">
+        <v>372.571</v>
+      </c>
+      <c r="O50" t="n">
+        <v>0.007</v>
+      </c>
       <c r="P50" t="s">
         <v>331</v>
       </c>
@@ -5021,7 +5048,7 @@
         <v>336</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D51" t="s">
         <v>337</v>
@@ -5033,31 +5060,31 @@
         <v>339</v>
       </c>
       <c r="G51" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="H51" t="n">
-        <v>13850</v>
+        <v>16309</v>
       </c>
       <c r="I51" t="n">
-        <v>0.475</v>
+        <v>0.56</v>
       </c>
       <c r="J51" t="n">
-        <v>210</v>
+        <v>817</v>
       </c>
       <c r="K51" t="n">
-        <v>0.007</v>
+        <v>0.028</v>
       </c>
       <c r="L51" t="n">
-        <v>250.667</v>
+        <v>737.667</v>
       </c>
       <c r="M51" t="n">
-        <v>0.008</v>
+        <v>0.025</v>
       </c>
       <c r="N51" t="n">
-        <v>434.714</v>
+        <v>458.714</v>
       </c>
       <c r="O51" t="n">
-        <v>0.015</v>
+        <v>0.016</v>
       </c>
       <c r="P51" t="s">
         <v>338</v>
@@ -5080,7 +5107,7 @@
         <v>343</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D52" t="s">
         <v>344</v>
@@ -5090,22 +5117,26 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H52" t="n">
-        <v>243277</v>
+        <v>254456</v>
       </c>
       <c r="I52" t="n">
-        <v>14.198</v>
+        <v>14.85</v>
       </c>
       <c r="J52" t="n">
-        <v>2717</v>
+        <v>4442</v>
       </c>
       <c r="K52" t="n">
-        <v>0.159</v>
-      </c>
-      <c r="L52"/>
-      <c r="M52"/>
+        <v>0.259</v>
+      </c>
+      <c r="L52" t="n">
+        <v>4035.667</v>
+      </c>
+      <c r="M52" t="n">
+        <v>0.235</v>
+      </c>
       <c r="N52"/>
       <c r="O52"/>
       <c r="P52" t="s">
@@ -5129,7 +5160,7 @@
         <v>350</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D53" t="s">
         <v>351</v>
@@ -5139,31 +5170,31 @@
       </c>
       <c r="F53"/>
       <c r="G53" t="n">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H53" t="n">
-        <v>160700</v>
+        <v>190326</v>
       </c>
       <c r="I53" t="n">
-        <v>33.325</v>
+        <v>39.468</v>
       </c>
       <c r="J53" t="n">
-        <v>4772</v>
+        <v>7287</v>
       </c>
       <c r="K53" t="n">
-        <v>0.99</v>
+        <v>1.511</v>
       </c>
       <c r="L53" t="n">
-        <v>3492.333</v>
+        <v>7434.333</v>
       </c>
       <c r="M53" t="n">
-        <v>0.724</v>
+        <v>1.542</v>
       </c>
       <c r="N53" t="n">
-        <v>4571</v>
+        <v>5729</v>
       </c>
       <c r="O53" t="n">
-        <v>0.948</v>
+        <v>1.188</v>
       </c>
       <c r="P53" t="s">
         <v>352</v>
@@ -5186,7 +5217,7 @@
         <v>355</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D54" t="s">
         <v>356</v>
@@ -5196,22 +5227,22 @@
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H54" t="n">
-        <v>21208</v>
+        <v>23835</v>
       </c>
       <c r="I54" t="n">
-        <v>0.103</v>
+        <v>0.116</v>
       </c>
       <c r="J54" t="n">
-        <v>1696</v>
+        <v>1343</v>
       </c>
       <c r="K54" t="n">
-        <v>0.008</v>
+        <v>0.007</v>
       </c>
       <c r="L54" t="n">
-        <v>1540</v>
+        <v>1441</v>
       </c>
       <c r="M54" t="n">
         <v>0.007</v>
@@ -5239,7 +5270,7 @@
         <v>361</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D55" t="s">
         <v>362</v>
@@ -5249,16 +5280,20 @@
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H55" t="n">
-        <v>188236</v>
+        <v>195921</v>
       </c>
       <c r="I55" t="n">
-        <v>34.722</v>
-      </c>
-      <c r="J55"/>
-      <c r="K55"/>
+        <v>36.14</v>
+      </c>
+      <c r="J55" t="n">
+        <v>3975</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0.733</v>
+      </c>
       <c r="L55"/>
       <c r="M55"/>
       <c r="N55"/>
@@ -5284,7 +5319,7 @@
         <v>368</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>43957</v>
+        <v>43961</v>
       </c>
       <c r="D56" t="s">
         <v>369</v>
@@ -5294,31 +5329,31 @@
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H56" t="n">
-        <v>232582</v>
+        <v>283517</v>
       </c>
       <c r="I56" t="n">
-        <v>1.053</v>
+        <v>1.284</v>
       </c>
       <c r="J56" t="n">
-        <v>10178</v>
+        <v>13492</v>
       </c>
       <c r="K56" t="n">
-        <v>0.046</v>
+        <v>0.061</v>
       </c>
       <c r="L56" t="n">
-        <v>9852.333</v>
+        <v>12913</v>
       </c>
       <c r="M56" t="n">
-        <v>0.045</v>
+        <v>0.058</v>
       </c>
       <c r="N56" t="n">
-        <v>9524.429</v>
+        <v>11498.857</v>
       </c>
       <c r="O56" t="n">
-        <v>0.043</v>
+        <v>0.052</v>
       </c>
       <c r="P56" t="s">
         <v>370</v>
@@ -5341,7 +5376,7 @@
         <v>374</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D57" t="s">
         <v>375</v>
@@ -5353,31 +5388,31 @@
         <v>376</v>
       </c>
       <c r="G57" t="n">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H57" t="n">
-        <v>36483</v>
+        <v>41649</v>
       </c>
       <c r="I57" t="n">
-        <v>8.455</v>
+        <v>9.653</v>
       </c>
       <c r="J57" t="n">
-        <v>927</v>
+        <v>1293</v>
       </c>
       <c r="K57" t="n">
-        <v>0.215</v>
+        <v>0.3</v>
       </c>
       <c r="L57" t="n">
-        <v>1043</v>
+        <v>1211.667</v>
       </c>
       <c r="M57" t="n">
-        <v>0.242</v>
+        <v>0.281</v>
       </c>
       <c r="N57" t="n">
-        <v>1098.286</v>
+        <v>1185</v>
       </c>
       <c r="O57" t="n">
-        <v>0.254</v>
+        <v>0.275</v>
       </c>
       <c r="P57" t="s">
         <v>43</v>
@@ -5400,7 +5435,7 @@
         <v>380</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D58" t="s">
         <v>381</v>
@@ -5412,31 +5447,31 @@
         <v>383</v>
       </c>
       <c r="G58" t="n">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="H58" t="n">
-        <v>11898</v>
+        <v>14646</v>
       </c>
       <c r="I58" t="n">
-        <v>1.668</v>
+        <v>2.053</v>
       </c>
       <c r="J58" t="n">
-        <v>458</v>
+        <v>800</v>
       </c>
       <c r="K58" t="n">
-        <v>0.064</v>
+        <v>0.112</v>
       </c>
       <c r="L58" t="n">
-        <v>382.333</v>
+        <v>716.333</v>
       </c>
       <c r="M58" t="n">
-        <v>0.054</v>
+        <v>0.1</v>
       </c>
       <c r="N58" t="n">
-        <v>431.714</v>
+        <v>554.286</v>
       </c>
       <c r="O58" t="n">
-        <v>0.061</v>
+        <v>0.078</v>
       </c>
       <c r="P58" t="s">
         <v>384</v>
@@ -5459,7 +5494,7 @@
         <v>388</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>43956</v>
+        <v>43961</v>
       </c>
       <c r="D59" t="s">
         <v>389</v>
@@ -5469,20 +5504,16 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H59" t="n">
-        <v>406579</v>
+        <v>494250</v>
       </c>
       <c r="I59" t="n">
-        <v>12.331</v>
-      </c>
-      <c r="J59" t="n">
-        <v>21087</v>
-      </c>
-      <c r="K59" t="n">
-        <v>0.64</v>
-      </c>
+        <v>14.99</v>
+      </c>
+      <c r="J59"/>
+      <c r="K59"/>
       <c r="L59"/>
       <c r="M59"/>
       <c r="N59"/>
@@ -5508,7 +5539,7 @@
         <v>395</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>43955</v>
+        <v>43958</v>
       </c>
       <c r="D60" t="s">
         <v>396</v>
@@ -5518,22 +5549,26 @@
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H60" t="n">
-        <v>119512</v>
+        <v>136706</v>
       </c>
       <c r="I60" t="n">
-        <v>1.091</v>
+        <v>1.248</v>
       </c>
       <c r="J60" t="n">
-        <v>6179</v>
+        <v>5216</v>
       </c>
       <c r="K60" t="n">
-        <v>0.056</v>
-      </c>
-      <c r="L60"/>
-      <c r="M60"/>
+        <v>0.048</v>
+      </c>
+      <c r="L60" t="n">
+        <v>5731.333</v>
+      </c>
+      <c r="M60" t="n">
+        <v>0.053</v>
+      </c>
       <c r="N60"/>
       <c r="O60"/>
       <c r="P60" t="s">
@@ -5557,7 +5592,7 @@
         <v>400</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D61" t="s">
         <v>401</v>
@@ -5569,31 +5604,31 @@
         <v>403</v>
       </c>
       <c r="G61" t="n">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H61" t="n">
-        <v>410468</v>
+        <v>460686</v>
       </c>
       <c r="I61" t="n">
-        <v>10.846</v>
+        <v>12.172</v>
       </c>
       <c r="J61" t="n">
-        <v>16198</v>
+        <v>17180</v>
       </c>
       <c r="K61" t="n">
-        <v>0.428</v>
+        <v>0.454</v>
       </c>
       <c r="L61" t="n">
-        <v>11506.667</v>
+        <v>16739.333</v>
       </c>
       <c r="M61" t="n">
-        <v>0.304</v>
+        <v>0.442</v>
       </c>
       <c r="N61" t="n">
-        <v>12277.286</v>
+        <v>13524.714</v>
       </c>
       <c r="O61" t="n">
-        <v>0.325</v>
+        <v>0.358</v>
       </c>
       <c r="P61" t="s">
         <v>404</v>
@@ -5616,7 +5651,7 @@
         <v>408</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>43955</v>
+        <v>43956</v>
       </c>
       <c r="D62" t="s">
         <v>409</v>
@@ -5626,31 +5661,31 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H62" t="n">
-        <v>470234</v>
+        <v>485925</v>
       </c>
       <c r="I62" t="n">
-        <v>46.116</v>
+        <v>47.655</v>
       </c>
       <c r="J62" t="n">
-        <v>11532</v>
+        <v>15556</v>
       </c>
       <c r="K62" t="n">
-        <v>1.131</v>
+        <v>1.526</v>
       </c>
       <c r="L62" t="n">
-        <v>10172.333</v>
+        <v>11893.667</v>
       </c>
       <c r="M62" t="n">
-        <v>0.997</v>
+        <v>1.166</v>
       </c>
       <c r="N62" t="n">
-        <v>12808.857</v>
+        <v>12837.714</v>
       </c>
       <c r="O62" t="n">
-        <v>1.256</v>
+        <v>1.259</v>
       </c>
       <c r="P62" t="s">
         <v>410</v>
@@ -5673,7 +5708,7 @@
         <v>414</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>43957</v>
+        <v>43961</v>
       </c>
       <c r="D63" t="s">
         <v>415</v>
@@ -5683,31 +5718,31 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H63" t="n">
-        <v>112963</v>
+        <v>127769</v>
       </c>
       <c r="I63" t="n">
-        <v>39.209</v>
+        <v>44.348</v>
       </c>
       <c r="J63" t="n">
-        <v>3201</v>
+        <v>3215</v>
       </c>
       <c r="K63" t="n">
-        <v>1.111</v>
+        <v>1.116</v>
       </c>
       <c r="L63" t="n">
-        <v>2842.667</v>
+        <v>3758</v>
       </c>
       <c r="M63" t="n">
-        <v>0.987</v>
+        <v>1.305</v>
       </c>
       <c r="N63" t="n">
-        <v>3078.286</v>
+        <v>3333.429</v>
       </c>
       <c r="O63" t="n">
-        <v>1.069</v>
+        <v>1.157</v>
       </c>
       <c r="P63" t="s">
         <v>416</v>
@@ -5730,7 +5765,7 @@
         <v>420</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D64" t="s">
         <v>421</v>
@@ -5742,31 +5777,31 @@
         <v>423</v>
       </c>
       <c r="G64" t="n">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="H64" t="n">
-        <v>217139</v>
+        <v>248056</v>
       </c>
       <c r="I64" t="n">
-        <v>11.287</v>
+        <v>12.894</v>
       </c>
       <c r="J64" t="n">
-        <v>11297</v>
+        <v>10776</v>
       </c>
       <c r="K64" t="n">
-        <v>0.587</v>
+        <v>0.56</v>
       </c>
       <c r="L64" t="n">
-        <v>7210.333</v>
+        <v>10305.667</v>
       </c>
       <c r="M64" t="n">
-        <v>0.375</v>
+        <v>0.535</v>
       </c>
       <c r="N64" t="n">
-        <v>7163.714</v>
+        <v>8216.571</v>
       </c>
       <c r="O64" t="n">
-        <v>0.372</v>
+        <v>0.427</v>
       </c>
       <c r="P64" t="s">
         <v>422</v>
@@ -5789,7 +5824,7 @@
         <v>426</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>43957</v>
+        <v>43961</v>
       </c>
       <c r="D65" t="s">
         <v>427</v>
@@ -5799,31 +5834,31 @@
       </c>
       <c r="F65"/>
       <c r="G65" t="n">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H65" t="n">
-        <v>4633731</v>
+        <v>5448463</v>
       </c>
       <c r="I65" t="n">
-        <v>31.752</v>
+        <v>37.335</v>
       </c>
       <c r="J65" t="n">
-        <v>173374</v>
+        <v>226499</v>
       </c>
       <c r="K65" t="n">
-        <v>1.188</v>
+        <v>1.552</v>
       </c>
       <c r="L65" t="n">
-        <v>177910.667</v>
+        <v>215090.333</v>
       </c>
       <c r="M65" t="n">
-        <v>1.219</v>
+        <v>1.474</v>
       </c>
       <c r="N65" t="n">
-        <v>190002</v>
+        <v>192637.714</v>
       </c>
       <c r="O65" t="n">
-        <v>1.302</v>
+        <v>1.32</v>
       </c>
       <c r="P65" t="s">
         <v>428</v>
@@ -5846,7 +5881,7 @@
         <v>432</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D66" t="s">
         <v>433</v>
@@ -5856,28 +5891,28 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H66" t="n">
-        <v>35992</v>
+        <v>41385</v>
       </c>
       <c r="I66" t="n">
-        <v>2.779</v>
+        <v>3.195</v>
       </c>
       <c r="J66" t="n">
-        <v>896</v>
+        <v>1198</v>
       </c>
       <c r="K66" t="n">
-        <v>0.069</v>
+        <v>0.092</v>
       </c>
       <c r="L66" t="n">
-        <v>896.333</v>
+        <v>1356.667</v>
       </c>
       <c r="M66" t="n">
-        <v>0.069</v>
+        <v>0.104</v>
       </c>
       <c r="N66" t="n">
-        <v>1156.571</v>
+        <v>1154.571</v>
       </c>
       <c r="O66" t="n">
         <v>0.089</v>
@@ -5903,7 +5938,7 @@
         <v>438</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D67" t="s">
         <v>439</v>
@@ -5913,18 +5948,26 @@
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H67" t="n">
-        <v>389659</v>
+        <v>433500</v>
       </c>
       <c r="I67" t="n">
-        <v>11.193</v>
-      </c>
-      <c r="J67"/>
-      <c r="K67"/>
-      <c r="L67"/>
-      <c r="M67"/>
+        <v>12.452</v>
+      </c>
+      <c r="J67" t="n">
+        <v>14778</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0.424</v>
+      </c>
+      <c r="L67" t="n">
+        <v>14613.667</v>
+      </c>
+      <c r="M67" t="n">
+        <v>0.419</v>
+      </c>
       <c r="N67"/>
       <c r="O67"/>
       <c r="P67" t="s">
@@ -5948,7 +5991,7 @@
         <v>442</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D68" t="s">
         <v>443</v>
@@ -5960,31 +6003,31 @@
         <v>445</v>
       </c>
       <c r="G68" t="n">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H68" t="n">
-        <v>17461</v>
+        <v>20217</v>
       </c>
       <c r="I68" t="n">
-        <v>1.043</v>
+        <v>1.207</v>
       </c>
       <c r="J68" t="n">
-        <v>1182</v>
+        <v>848</v>
       </c>
       <c r="K68" t="n">
-        <v>0.071</v>
+        <v>0.051</v>
       </c>
       <c r="L68" t="n">
-        <v>897</v>
+        <v>915.667</v>
       </c>
       <c r="M68" t="n">
-        <v>0.054</v>
+        <v>0.055</v>
       </c>
       <c r="N68" t="n">
-        <v>964.714</v>
+        <v>892.571</v>
       </c>
       <c r="O68" t="n">
-        <v>0.058</v>
+        <v>0.053</v>
       </c>
       <c r="P68" t="s">
         <v>446</v>
@@ -6007,7 +6050,7 @@
         <v>451</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D69" t="s">
         <v>452</v>
@@ -6019,31 +6062,31 @@
         <v>453</v>
       </c>
       <c r="G69" t="n">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H69" t="n">
-        <v>117474</v>
+        <v>134533</v>
       </c>
       <c r="I69" t="n">
-        <v>17.264</v>
+        <v>19.771</v>
       </c>
       <c r="J69" t="n">
-        <v>6196</v>
+        <v>5728</v>
       </c>
       <c r="K69" t="n">
-        <v>0.911</v>
+        <v>0.842</v>
       </c>
       <c r="L69" t="n">
-        <v>5187.667</v>
+        <v>5686.333</v>
       </c>
       <c r="M69" t="n">
-        <v>0.763</v>
+        <v>0.836</v>
       </c>
       <c r="N69" t="n">
-        <v>5504.571</v>
+        <v>5413.714</v>
       </c>
       <c r="O69" t="n">
-        <v>0.809</v>
+        <v>0.796</v>
       </c>
       <c r="P69" t="s">
         <v>43</v>
@@ -6156,7 +6199,7 @@
         <v>465</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>43957</v>
+        <v>43961</v>
       </c>
       <c r="D72" t="s">
         <v>466</v>
@@ -6166,31 +6209,25 @@
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="H72" t="n">
-        <v>104606</v>
+        <v>119859</v>
       </c>
       <c r="I72" t="n">
-        <v>19.16</v>
-      </c>
-      <c r="J72" t="n">
-        <v>4742</v>
-      </c>
+        <v>21.954</v>
+      </c>
+      <c r="J72"/>
       <c r="K72" t="n">
-        <v>0.869</v>
-      </c>
-      <c r="L72" t="n">
-        <v>2795.333</v>
-      </c>
+        <v>0.273</v>
+      </c>
+      <c r="L72"/>
       <c r="M72" t="n">
-        <v>0.512</v>
-      </c>
-      <c r="N72" t="n">
-        <v>3324</v>
-      </c>
+        <v>0.616</v>
+      </c>
+      <c r="N72"/>
       <c r="O72" t="n">
-        <v>0.609</v>
+        <v>0.619</v>
       </c>
       <c r="P72" t="s">
         <v>468</v>
@@ -6213,7 +6250,7 @@
         <v>473</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D73" t="s">
         <v>474</v>
@@ -6223,31 +6260,31 @@
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H73" t="n">
-        <v>58923</v>
+        <v>62828</v>
       </c>
       <c r="I73" t="n">
-        <v>28.343</v>
+        <v>30.221</v>
       </c>
       <c r="J73" t="n">
-        <v>1449</v>
+        <v>625</v>
       </c>
       <c r="K73" t="n">
-        <v>0.697</v>
+        <v>0.301</v>
       </c>
       <c r="L73" t="n">
-        <v>1134.333</v>
+        <v>950</v>
       </c>
       <c r="M73" t="n">
-        <v>0.546</v>
+        <v>0.457</v>
       </c>
       <c r="N73" t="n">
-        <v>1045.143</v>
+        <v>1044</v>
       </c>
       <c r="O73" t="n">
-        <v>0.503</v>
+        <v>0.502</v>
       </c>
       <c r="P73" t="s">
         <v>476</v>
@@ -6270,7 +6307,7 @@
         <v>480</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D74" t="s">
         <v>481</v>
@@ -6282,31 +6319,31 @@
         <v>483</v>
       </c>
       <c r="G74" t="n">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H74" t="n">
-        <v>268064</v>
+        <v>324079</v>
       </c>
       <c r="I74" t="n">
-        <v>4.52</v>
+        <v>5.464</v>
       </c>
       <c r="J74" t="n">
-        <v>10523</v>
+        <v>16327</v>
       </c>
       <c r="K74" t="n">
-        <v>0.177</v>
+        <v>0.275</v>
       </c>
       <c r="L74" t="n">
-        <v>12459.333</v>
+        <v>14900</v>
       </c>
       <c r="M74" t="n">
-        <v>0.21</v>
+        <v>0.251</v>
       </c>
       <c r="N74" t="n">
-        <v>11795.286</v>
+        <v>13341.857</v>
       </c>
       <c r="O74" t="n">
-        <v>0.199</v>
+        <v>0.225</v>
       </c>
       <c r="P74" t="s">
         <v>482</v>
@@ -6329,7 +6366,7 @@
         <v>487</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>43957</v>
+        <v>43961</v>
       </c>
       <c r="D75" t="s">
         <v>488</v>
@@ -6339,25 +6376,31 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="H75" t="n">
-        <v>643095</v>
+        <v>663886</v>
       </c>
       <c r="I75" t="n">
-        <v>12.544</v>
-      </c>
-      <c r="J75"/>
+        <v>12.949</v>
+      </c>
+      <c r="J75" t="n">
+        <v>3856</v>
+      </c>
       <c r="K75" t="n">
-        <v>0.056</v>
-      </c>
-      <c r="L75"/>
+        <v>0.075</v>
+      </c>
+      <c r="L75" t="n">
+        <v>4832.667</v>
+      </c>
       <c r="M75" t="n">
-        <v>0.079</v>
-      </c>
-      <c r="N75"/>
+        <v>0.094</v>
+      </c>
+      <c r="N75" t="n">
+        <v>4701.857</v>
+      </c>
       <c r="O75" t="n">
-        <v>0.081</v>
+        <v>0.092</v>
       </c>
       <c r="P75" t="s">
         <v>489</v>
@@ -6380,7 +6423,7 @@
         <v>493</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>43951</v>
+        <v>43958</v>
       </c>
       <c r="D76" t="s">
         <v>494</v>
@@ -6388,15 +6431,17 @@
       <c r="E76" t="s">
         <v>495</v>
       </c>
-      <c r="F76"/>
+      <c r="F76" t="s">
+        <v>496</v>
+      </c>
       <c r="G76" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H76" t="n">
-        <v>1351130</v>
+        <v>1625211</v>
       </c>
       <c r="I76" t="n">
-        <v>28.898</v>
+        <v>34.76</v>
       </c>
       <c r="J76"/>
       <c r="K76"/>
@@ -6405,33 +6450,33 @@
       <c r="N76"/>
       <c r="O76"/>
       <c r="P76" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="Q76" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="R76" t="s">
         <v>24</v>
       </c>
       <c r="S76" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B77" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C77" s="1" t="n">
         <v>43954</v>
       </c>
       <c r="D77" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="E77" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
@@ -6450,61 +6495,61 @@
       <c r="N77"/>
       <c r="O77"/>
       <c r="P77" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q77" t="s">
         <v>502</v>
-      </c>
-      <c r="Q77" t="s">
-        <v>501</v>
       </c>
       <c r="R77" t="s">
         <v>94</v>
       </c>
       <c r="S77" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B78" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D78" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E78" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="H78" t="n">
-        <v>290365</v>
+        <v>309595</v>
       </c>
       <c r="I78" t="n">
-        <v>33.55</v>
+        <v>35.772</v>
       </c>
       <c r="J78"/>
       <c r="K78" t="n">
-        <v>0.153</v>
+        <v>0.045</v>
       </c>
       <c r="L78"/>
       <c r="M78" t="n">
-        <v>0.272</v>
+        <v>0.336</v>
       </c>
       <c r="N78"/>
       <c r="O78" t="n">
-        <v>0.419</v>
+        <v>0.434</v>
       </c>
       <c r="P78" t="s">
         <v>508</v>
       </c>
       <c r="Q78" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="R78" t="s">
         <v>509</v>
@@ -6521,7 +6566,7 @@
         <v>512</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D79" t="s">
         <v>513</v>
@@ -6531,31 +6576,31 @@
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H79" t="n">
-        <v>65589</v>
+        <v>67133</v>
       </c>
       <c r="I79" t="n">
-        <v>2.754</v>
+        <v>2.819</v>
       </c>
       <c r="J79" t="n">
-        <v>631</v>
+        <v>272</v>
       </c>
       <c r="K79" t="n">
-        <v>0.026</v>
+        <v>0.011</v>
       </c>
       <c r="L79" t="n">
-        <v>498.333</v>
+        <v>362.333</v>
       </c>
       <c r="M79" t="n">
-        <v>0.021</v>
+        <v>0.015</v>
       </c>
       <c r="N79" t="n">
-        <v>460.143</v>
+        <v>434.143</v>
       </c>
       <c r="O79" t="n">
-        <v>0.019</v>
+        <v>0.018</v>
       </c>
       <c r="P79" t="s">
         <v>514</v>
@@ -6578,7 +6623,7 @@
         <v>519</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>43957</v>
+        <v>43961</v>
       </c>
       <c r="D80" t="s">
         <v>520</v>
@@ -6588,31 +6633,25 @@
       </c>
       <c r="F80"/>
       <c r="G80" t="n">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H80" t="n">
-        <v>86320</v>
+        <v>97177</v>
       </c>
       <c r="I80" t="n">
-        <v>1.237</v>
-      </c>
-      <c r="J80" t="n">
-        <v>3693</v>
-      </c>
+        <v>1.392</v>
+      </c>
+      <c r="J80"/>
       <c r="K80" t="n">
-        <v>0.053</v>
-      </c>
-      <c r="L80" t="n">
-        <v>3684</v>
-      </c>
+        <v>0.003</v>
+      </c>
+      <c r="L80"/>
       <c r="M80" t="n">
-        <v>0.053</v>
-      </c>
-      <c r="N80" t="n">
-        <v>3471.714</v>
-      </c>
+        <v>0.035</v>
+      </c>
+      <c r="N80"/>
       <c r="O80" t="n">
-        <v>0.05</v>
+        <v>0.045</v>
       </c>
       <c r="P80" t="s">
         <v>522</v>
@@ -6635,7 +6674,7 @@
         <v>526</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>43955</v>
+        <v>43958</v>
       </c>
       <c r="D81" t="s">
         <v>527</v>
@@ -6645,32 +6684,20 @@
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H81" t="n">
-        <v>25165</v>
+        <v>27420</v>
       </c>
       <c r="I81" t="n">
-        <v>2.129</v>
-      </c>
-      <c r="J81" t="n">
-        <v>312</v>
-      </c>
-      <c r="K81" t="n">
-        <v>0.026</v>
-      </c>
-      <c r="L81" t="n">
-        <v>370</v>
-      </c>
-      <c r="M81" t="n">
-        <v>0.031</v>
-      </c>
-      <c r="N81" t="n">
-        <v>526.857</v>
-      </c>
-      <c r="O81" t="n">
-        <v>0.045</v>
-      </c>
+        <v>2.32</v>
+      </c>
+      <c r="J81"/>
+      <c r="K81"/>
+      <c r="L81"/>
+      <c r="M81"/>
+      <c r="N81"/>
+      <c r="O81"/>
       <c r="P81" t="s">
         <v>528</v>
       </c>
@@ -6692,7 +6719,7 @@
         <v>533</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D82" t="s">
         <v>534</v>
@@ -6702,25 +6729,25 @@
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H82" t="n">
-        <v>1234724</v>
+        <v>1334411</v>
       </c>
       <c r="I82" t="n">
-        <v>14.64</v>
+        <v>15.822</v>
       </c>
       <c r="J82" t="n">
-        <v>30303</v>
+        <v>35605</v>
       </c>
       <c r="K82" t="n">
-        <v>0.359</v>
+        <v>0.422</v>
       </c>
       <c r="L82" t="n">
-        <v>33119</v>
+        <v>33229</v>
       </c>
       <c r="M82" t="n">
-        <v>0.393</v>
+        <v>0.394</v>
       </c>
       <c r="N82"/>
       <c r="O82"/>
@@ -6745,7 +6772,7 @@
         <v>540</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>43956</v>
+        <v>43959</v>
       </c>
       <c r="D83" t="s">
         <v>541</v>
@@ -6757,31 +6784,31 @@
         <v>543</v>
       </c>
       <c r="G83" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H83" t="n">
-        <v>44094</v>
+        <v>55203</v>
       </c>
       <c r="I83" t="n">
-        <v>0.964</v>
+        <v>1.207</v>
       </c>
       <c r="J83" t="n">
-        <v>2632</v>
+        <v>3161</v>
       </c>
       <c r="K83" t="n">
-        <v>0.058</v>
+        <v>0.069</v>
       </c>
       <c r="L83" t="n">
-        <v>2602.667</v>
+        <v>3493</v>
       </c>
       <c r="M83" t="n">
-        <v>0.057</v>
+        <v>0.076</v>
       </c>
       <c r="N83" t="n">
-        <v>2402.714</v>
+        <v>2967.286</v>
       </c>
       <c r="O83" t="n">
-        <v>0.053</v>
+        <v>0.065</v>
       </c>
       <c r="P83" t="s">
         <v>542</v>
@@ -6804,7 +6831,7 @@
         <v>547</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>43957</v>
+        <v>43961</v>
       </c>
       <c r="D84" t="s">
         <v>548</v>
@@ -6814,31 +6841,31 @@
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H84" t="n">
-        <v>144283</v>
+        <v>176403</v>
       </c>
       <c r="I84" t="n">
-        <v>3.299</v>
+        <v>4.034</v>
       </c>
       <c r="J84" t="n">
-        <v>4524</v>
+        <v>9296</v>
       </c>
       <c r="K84" t="n">
-        <v>0.103</v>
+        <v>0.213</v>
       </c>
       <c r="L84" t="n">
-        <v>4853.333</v>
+        <v>8278</v>
       </c>
       <c r="M84" t="n">
-        <v>0.111</v>
+        <v>0.189</v>
       </c>
       <c r="N84" t="n">
-        <v>5677</v>
+        <v>6668.571</v>
       </c>
       <c r="O84" t="n">
-        <v>0.13</v>
+        <v>0.152</v>
       </c>
       <c r="P84" t="s">
         <v>549</v>
@@ -6861,7 +6888,7 @@
         <v>554</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D85" t="s">
         <v>555</v>
@@ -6871,31 +6898,31 @@
       </c>
       <c r="F85"/>
       <c r="G85" t="n">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H85" t="n">
-        <v>1072144</v>
+        <v>1270408</v>
       </c>
       <c r="I85" t="n">
-        <v>15.793</v>
+        <v>18.714</v>
       </c>
       <c r="J85" t="n">
-        <v>57006</v>
+        <v>63339</v>
       </c>
       <c r="K85" t="n">
-        <v>0.84</v>
+        <v>0.933</v>
       </c>
       <c r="L85" t="n">
-        <v>63267</v>
+        <v>65291.333</v>
       </c>
       <c r="M85" t="n">
-        <v>0.932</v>
+        <v>0.962</v>
       </c>
       <c r="N85" t="n">
-        <v>62518.714</v>
+        <v>63153.143</v>
       </c>
       <c r="O85" t="n">
-        <v>0.921</v>
+        <v>0.93</v>
       </c>
       <c r="P85" t="s">
         <v>556</v>
@@ -6918,7 +6945,7 @@
         <v>559</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D86" t="s">
         <v>560</v>
@@ -6928,31 +6955,31 @@
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H86" t="n">
-        <v>1448010</v>
+        <v>1728443</v>
       </c>
       <c r="I86" t="n">
-        <v>21.33</v>
+        <v>25.461</v>
       </c>
       <c r="J86" t="n">
-        <v>69463</v>
+        <v>96878</v>
       </c>
       <c r="K86" t="n">
-        <v>1.023</v>
+        <v>1.427</v>
       </c>
       <c r="L86" t="n">
-        <v>79818.333</v>
+        <v>93496.667</v>
       </c>
       <c r="M86" t="n">
-        <v>1.176</v>
+        <v>1.377</v>
       </c>
       <c r="N86" t="n">
-        <v>89406.571</v>
+        <v>85205.857</v>
       </c>
       <c r="O86" t="n">
-        <v>1.317</v>
+        <v>1.255</v>
       </c>
       <c r="P86" t="s">
         <v>556</v>
@@ -6975,7 +7002,7 @@
         <v>564</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D87" t="s">
         <v>565</v>
@@ -6985,31 +7012,31 @@
       </c>
       <c r="F87"/>
       <c r="G87" t="n">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H87" t="n">
-        <v>7544328</v>
+        <v>8709630</v>
       </c>
       <c r="I87" t="n">
-        <v>22.792</v>
+        <v>26.313</v>
       </c>
       <c r="J87" t="n">
-        <v>258954</v>
+        <v>300842</v>
       </c>
       <c r="K87" t="n">
-        <v>0.782</v>
+        <v>0.909</v>
       </c>
       <c r="L87" t="n">
-        <v>246362.333</v>
+        <v>307612.333</v>
       </c>
       <c r="M87" t="n">
-        <v>0.744</v>
+        <v>0.929</v>
       </c>
       <c r="N87" t="n">
-        <v>249771.857</v>
+        <v>272055.571</v>
       </c>
       <c r="O87" t="n">
-        <v>0.755</v>
+        <v>0.822</v>
       </c>
       <c r="P87" t="s">
         <v>566</v>
@@ -7032,7 +7059,7 @@
         <v>570</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>43949</v>
+        <v>43952</v>
       </c>
       <c r="D88" t="s">
         <v>571</v>
@@ -7042,31 +7069,31 @@
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H88" t="n">
-        <v>606361</v>
+        <v>695283</v>
       </c>
       <c r="I88" t="n">
-        <v>1.832</v>
+        <v>2.101</v>
       </c>
       <c r="J88" t="n">
-        <v>23063</v>
+        <v>23633</v>
       </c>
       <c r="K88" t="n">
-        <v>0.07</v>
+        <v>0.071</v>
       </c>
       <c r="L88" t="n">
-        <v>18202.667</v>
+        <v>24423.333</v>
       </c>
       <c r="M88" t="n">
-        <v>0.055</v>
+        <v>0.074</v>
       </c>
       <c r="N88" t="n">
-        <v>19781.714</v>
+        <v>21015.714</v>
       </c>
       <c r="O88" t="n">
-        <v>0.06</v>
+        <v>0.063</v>
       </c>
       <c r="P88" t="s">
         <v>573</v>
@@ -7089,7 +7116,7 @@
         <v>578</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>43957</v>
+        <v>43961</v>
       </c>
       <c r="D89" t="s">
         <v>579</v>
@@ -7099,31 +7126,31 @@
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H89" t="n">
-        <v>23811</v>
+        <v>27461</v>
       </c>
       <c r="I89" t="n">
-        <v>6.855</v>
+        <v>7.905</v>
       </c>
       <c r="J89" t="n">
-        <v>1006</v>
+        <v>623</v>
       </c>
       <c r="K89" t="n">
-        <v>0.29</v>
+        <v>0.179</v>
       </c>
       <c r="L89" t="n">
-        <v>882.333</v>
+        <v>935</v>
       </c>
       <c r="M89" t="n">
-        <v>0.254</v>
+        <v>0.269</v>
       </c>
       <c r="N89" t="n">
-        <v>810.143</v>
+        <v>899.571</v>
       </c>
       <c r="O89" t="n">
-        <v>0.233</v>
+        <v>0.259</v>
       </c>
       <c r="P89" t="s">
         <v>126</v>
@@ -7191,7 +7218,7 @@
         <v>590</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>43956</v>
+        <v>43959</v>
       </c>
       <c r="D91" t="s">
         <v>591</v>
@@ -7201,32 +7228,24 @@
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="H91" t="n">
-        <v>14821</v>
+        <v>8741</v>
       </c>
       <c r="I91" t="n">
-        <v>0.997</v>
+        <v>0.588</v>
       </c>
       <c r="J91" t="n">
-        <v>1492</v>
+        <v>600</v>
       </c>
       <c r="K91" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="L91" t="n">
-        <v>1364.667</v>
-      </c>
-      <c r="M91" t="n">
-        <v>0.092</v>
-      </c>
-      <c r="N91" t="n">
-        <v>1076.286</v>
-      </c>
-      <c r="O91" t="n">
-        <v>0.072</v>
-      </c>
+        <v>0.04</v>
+      </c>
+      <c r="L91"/>
+      <c r="M91"/>
+      <c r="N91"/>
+      <c r="O91"/>
       <c r="P91" t="s">
         <v>592</v>
       </c>

</xml_diff>